<commit_message>
commit for code pull
</commit_message>
<xml_diff>
--- a/target/test-classes/testData/Test_Data_Sheet.xlsx
+++ b/target/test-classes/testData/Test_Data_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT_Automation\WorkSpace\Selenium_Training_B16\Selenium_Training_B16_MVN\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DAAC57-5493-4D42-896D-D1FA82ED4747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0812C91E-7EC1-46A8-9600-ABB559E60A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Test_Data" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Test_Cases!$A$1:$E$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Test_Cases!$A$1:$E$11</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -660,10 +660,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -710,7 +711,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -727,7 +728,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -735,7 +736,7 @@
         <v>43</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>51</v>
@@ -752,7 +753,7 @@
         <v>44</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>49</v>
@@ -761,7 +762,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -769,7 +770,7 @@
         <v>45</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>50</v>
@@ -778,7 +779,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -803,7 +804,7 @@
         <v>55</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>49</v>
@@ -812,7 +813,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -829,7 +830,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -854,7 +855,7 @@
         <v>58</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>49</v>
@@ -864,7 +865,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E7" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A1:E11" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Regression"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C11" xr:uid="{E3D1410E-F577-46E5-AF83-4F9B0549376C}">
@@ -879,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>